<commit_message>
Automatic push - Excel file Update
</commit_message>
<xml_diff>
--- a/Data/Historique d'achats.xlsx
+++ b/Data/Historique d'achats.xlsx
@@ -7732,11 +7732,11 @@
           </val>
         </ser>
         <marker val="1"/>
-        <axId val="72826880"/>
-        <axId val="72828800"/>
+        <axId val="71120768"/>
+        <axId val="71127040"/>
       </lineChart>
       <dateAx>
-        <axId val="72826880"/>
+        <axId val="71120768"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -7745,12 +7745,12 @@
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
-        <crossAx val="72828800"/>
+        <crossAx val="71127040"/>
         <crosses val="autoZero"/>
         <lblOffset val="100"/>
       </dateAx>
       <valAx>
-        <axId val="72828800"/>
+        <axId val="71127040"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -7760,7 +7760,7 @@
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
-        <crossAx val="72826880"/>
+        <crossAx val="71120768"/>
         <crosses val="autoZero"/>
         <crossBetween val="between"/>
       </valAx>
@@ -8197,7 +8197,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>2432.049779341159</v>
+        <v>2431.335117111788</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -8525,7 +8525,7 @@
     </row>
     <row r="12">
       <c r="B12" s="25" t="n">
-        <v>0.00709189</v>
+        <v>0.00709191</v>
       </c>
       <c r="C12" s="61" t="n">
         <v>0</v>
@@ -9349,7 +9349,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>1.394389722358165</v>
+        <v>1.395088987575467</v>
       </c>
     </row>
     <row r="4">
@@ -9451,7 +9451,7 @@
     </row>
     <row r="6">
       <c r="B6" s="81" t="n">
-        <v>0.59778748</v>
+        <v>0.5977881900000001</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -9732,7 +9732,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>9.497660095266127</v>
+        <v>9.503314883651584</v>
       </c>
     </row>
     <row r="4">
@@ -9827,7 +9827,7 @@
     </row>
     <row r="7">
       <c r="B7" s="81" t="n">
-        <v>0.02860214</v>
+        <v>0.02860224</v>
       </c>
       <c r="C7" s="61" t="n">
         <v>0</v>
@@ -9987,7 +9987,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>35.38273794480155</v>
+        <v>35.44784459991394</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -10106,7 +10106,7 @@
     </row>
     <row r="6">
       <c r="B6" s="25" t="n">
-        <v>0.01664799</v>
+        <v>0.01664801</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -10640,7 +10640,7 @@
         </is>
       </c>
       <c r="J3" s="82" t="n">
-        <v>0.003535159906151476</v>
+        <v>0.003540437388861341</v>
       </c>
     </row>
     <row r="4">
@@ -11007,7 +11007,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>307.7119437597668</v>
+        <v>307.7784804309184</v>
       </c>
     </row>
     <row r="4">
@@ -11602,7 +11602,7 @@
         </is>
       </c>
       <c r="J3" s="85" t="n">
-        <v>0.07998435513640374</v>
+        <v>0.08001050228778817</v>
       </c>
     </row>
     <row r="4">
@@ -11664,7 +11664,7 @@
     </row>
     <row r="6">
       <c r="B6" s="81" t="n">
-        <v>0.28882871</v>
+        <v>0.2888292</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -11838,7 +11838,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>6.935247338872811</v>
+        <v>6.936090082813577</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -11957,7 +11957,7 @@
     </row>
     <row r="6">
       <c r="B6" s="25" t="n">
-        <v>0.07837002999999999</v>
+        <v>0.0783703</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -12326,7 +12326,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>53.41343187514222</v>
+        <v>53.44442799810887</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -12733,7 +12733,7 @@
         </is>
       </c>
       <c r="J3" s="79" t="n">
-        <v>0.1613075616783636</v>
+        <v>0.1612753629890426</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -13306,7 +13306,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>12.31223890735218</v>
+        <v>12.32566301716714</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -13755,7 +13755,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>44181.76393756232</v>
+        <v>44225.23836018965</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -15319,7 +15319,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>0.7103344537288785</v>
+        <v>0.7105861771675925</v>
       </c>
     </row>
     <row r="4">
@@ -15568,7 +15568,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>2.924812564735755</v>
+        <v>2.929678585441778</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -15684,7 +15684,7 @@
     </row>
     <row r="6">
       <c r="B6" s="2" t="n">
-        <v>0.01978546</v>
+        <v>0.01978558</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -15973,7 +15973,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>18.75162590265986</v>
+        <v>18.73806294101846</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -16364,7 +16364,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>68.7320825184664</v>
+        <v>68.73090757338211</v>
       </c>
       <c r="N3" s="24" t="n"/>
       <c r="O3" s="59" t="n"/>
@@ -16812,7 +16812,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>0.6602752266155621</v>
+        <v>0.6608173586844314</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -16886,7 +16886,7 @@
     </row>
     <row r="6">
       <c r="B6" s="84" t="n">
-        <v>0.05813364</v>
+        <v>0.0581337</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -17185,7 +17185,7 @@
         </is>
       </c>
       <c r="J3" s="67" t="n">
-        <v>0.0001080805644396994</v>
+        <v>0.0001083803173017418</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -17604,7 +17604,7 @@
     </row>
     <row r="18">
       <c r="B18" s="81" t="n">
-        <v>4984.76966369</v>
+        <v>4984.77854249</v>
       </c>
       <c r="C18" s="61" t="n">
         <v>0</v>
@@ -18056,7 +18056,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>0.8320005982940152</v>
+        <v>0.8320084746581266</v>
       </c>
       <c r="N3" s="19" t="n"/>
       <c r="O3" s="59" t="n"/>
@@ -18155,7 +18155,7 @@
     </row>
     <row r="6">
       <c r="B6" s="20" t="n">
-        <v>0.32762543</v>
+        <v>0.32762569</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -18608,8 +18608,8 @@
     <col width="9.140625" customWidth="1" style="14" min="10" max="13"/>
     <col width="10.140625" bestFit="1" customWidth="1" style="14" min="14" max="14"/>
     <col width="11.28515625" bestFit="1" customWidth="1" style="14" min="15" max="15"/>
-    <col width="9.140625" customWidth="1" style="14" min="16" max="337"/>
-    <col width="9.140625" customWidth="1" style="14" min="338" max="16384"/>
+    <col width="9.140625" customWidth="1" style="14" min="16" max="338"/>
+    <col width="9.140625" customWidth="1" style="14" min="339" max="16384"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -18621,7 +18621,7 @@
         </is>
       </c>
       <c r="J3" s="79" t="n">
-        <v>0.0226541587929937</v>
+        <v>0.02268818025768446</v>
       </c>
     </row>
     <row r="4">
@@ -18688,7 +18688,7 @@
     </row>
     <row r="6">
       <c r="B6" s="81" t="n">
-        <v>0.06628282000000001</v>
+        <v>0.06628315</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -18896,7 +18896,7 @@
         </is>
       </c>
       <c r="J3" s="79" t="n">
-        <v>1.182838898396509</v>
+        <v>1.18250092292378</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -19002,7 +19002,7 @@
     </row>
     <row r="6">
       <c r="B6" s="81" t="n">
-        <v>0.34820851</v>
+        <v>0.34820876</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -19404,7 +19404,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>2.878223464657085</v>
+        <v>2.883934190571152</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -19577,7 +19577,7 @@
     </row>
     <row r="7">
       <c r="B7" s="2" t="n">
-        <v>0.10241852</v>
+        <v>0.10241865</v>
       </c>
       <c r="C7" s="61" t="n">
         <v>0</v>
@@ -23551,8 +23551,8 @@
     <col width="9.140625" customWidth="1" style="14" min="10" max="13"/>
     <col width="10.140625" bestFit="1" customWidth="1" style="14" min="14" max="14"/>
     <col width="11.28515625" bestFit="1" customWidth="1" style="14" min="15" max="15"/>
-    <col width="9.140625" customWidth="1" style="14" min="16" max="358"/>
-    <col width="9.140625" customWidth="1" style="14" min="359" max="16384"/>
+    <col width="9.140625" customWidth="1" style="14" min="16" max="359"/>
+    <col width="9.140625" customWidth="1" style="14" min="360" max="16384"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -23580,7 +23580,7 @@
         </is>
       </c>
       <c r="J3" s="79" t="n">
-        <v>0.6294961726156207</v>
+        <v>0.6274692954273903</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -23686,7 +23686,7 @@
     </row>
     <row r="6">
       <c r="B6" s="81" t="n">
-        <v>0.07614131</v>
+        <v>0.07614136000000001</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -23955,7 +23955,7 @@
         </is>
       </c>
       <c r="J3" s="88" t="n">
-        <v>9.06526133879246e-06</v>
+        <v>9.065334467021332e-06</v>
       </c>
     </row>
     <row r="4">
@@ -24262,7 +24262,7 @@
         </is>
       </c>
       <c r="J3" s="82" t="n">
-        <v>0.003647745779920443</v>
+        <v>0.003628865493773073</v>
       </c>
     </row>
     <row r="4">
@@ -24486,7 +24486,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>100.2140468284386</v>
+        <v>100.5348418805912</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -25084,7 +25084,7 @@
     </row>
     <row r="17">
       <c r="B17" s="25" t="n">
-        <v>0.06440983</v>
+        <v>0.06440989</v>
       </c>
       <c r="C17" s="61" t="n">
         <v>0</v>
@@ -25980,7 +25980,7 @@
         </is>
       </c>
       <c r="J3" s="79" t="n">
-        <v>0.1246845777443642</v>
+        <v>0.124806874439672</v>
       </c>
     </row>
     <row r="4">
@@ -26044,7 +26044,7 @@
     </row>
     <row r="6">
       <c r="B6" s="20" t="n">
-        <v>0.26185895</v>
+        <v>0.26185983</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -26270,7 +26270,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>6.440387815282389</v>
+        <v>6.44687536251554</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -26394,7 +26394,7 @@
     </row>
     <row r="6">
       <c r="B6" s="2" t="n">
-        <v>0.00271741</v>
+        <v>0.00271742</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -26694,7 +26694,7 @@
         </is>
       </c>
       <c r="J3" s="79" t="n">
-        <v>0.5131238960389886</v>
+        <v>0.5129651902592521</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -26800,7 +26800,7 @@
     </row>
     <row r="6">
       <c r="B6" s="20" t="n">
-        <v>0.85428722</v>
+        <v>0.85428951</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -27078,8 +27078,8 @@
     <col width="11.28515625" bestFit="1" customWidth="1" style="14" min="15" max="15"/>
     <col width="9.140625" customWidth="1" style="14" min="16" max="19"/>
     <col width="10.28515625" bestFit="1" customWidth="1" style="14" min="20" max="20"/>
-    <col width="9.140625" customWidth="1" style="14" min="21" max="321"/>
-    <col width="9.140625" customWidth="1" style="14" min="322" max="16384"/>
+    <col width="9.140625" customWidth="1" style="14" min="21" max="322"/>
+    <col width="9.140625" customWidth="1" style="14" min="323" max="16384"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -27107,7 +27107,7 @@
         </is>
       </c>
       <c r="J3" s="79" t="n">
-        <v>18.65400970403573</v>
+        <v>18.68234781146852</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -27213,7 +27213,7 @@
     </row>
     <row r="6">
       <c r="B6" s="2" t="n">
-        <v>0.00314775</v>
+        <v>0.00314797</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -27446,8 +27446,8 @@
     <col width="11.28515625" bestFit="1" customWidth="1" style="14" min="15" max="15"/>
     <col width="9.140625" customWidth="1" style="14" min="16" max="19"/>
     <col width="10.28515625" bestFit="1" customWidth="1" style="14" min="20" max="20"/>
-    <col width="9.140625" customWidth="1" style="14" min="21" max="321"/>
-    <col width="9.140625" customWidth="1" style="14" min="322" max="16384"/>
+    <col width="9.140625" customWidth="1" style="14" min="21" max="322"/>
+    <col width="9.140625" customWidth="1" style="14" min="323" max="16384"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -27459,7 +27459,7 @@
         </is>
       </c>
       <c r="J3" s="79" t="n">
-        <v>2.869681944076967</v>
+        <v>2.88121615495917</v>
       </c>
       <c r="N3" s="19" t="n"/>
       <c r="O3" s="86" t="n"/>
@@ -27551,7 +27551,7 @@
     </row>
     <row r="6">
       <c r="B6" s="2" t="n">
-        <v>0.00064746</v>
+        <v>0.0006475</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -27753,7 +27753,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>0.3370376375779364</v>
+        <v>0.3374789294062976</v>
       </c>
     </row>
     <row r="4">
@@ -28193,7 +28193,7 @@
         </is>
       </c>
       <c r="J3" s="67" t="n">
-        <v>0.00413500825260368</v>
+        <v>0.004137509500077404</v>
       </c>
     </row>
     <row r="4">
@@ -30028,8 +30028,8 @@
     <col width="9.140625" customWidth="1" style="14" min="10" max="13"/>
     <col width="10.140625" bestFit="1" customWidth="1" style="14" min="14" max="14"/>
     <col width="11.28515625" bestFit="1" customWidth="1" style="14" min="15" max="15"/>
-    <col width="9.140625" customWidth="1" style="14" min="16" max="328"/>
-    <col width="9.140625" customWidth="1" style="14" min="329" max="16384"/>
+    <col width="9.140625" customWidth="1" style="14" min="16" max="329"/>
+    <col width="9.140625" customWidth="1" style="14" min="330" max="16384"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -30057,7 +30057,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>8.488047601101549</v>
+        <v>8.502654493311978</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -30433,7 +30433,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>0.4990480207355804</v>
+        <v>0.4990858220731613</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -30544,7 +30544,7 @@
     </row>
     <row r="6">
       <c r="B6" s="2" t="n">
-        <v>0.7714594299999999</v>
+        <v>0.77146149</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -30857,7 +30857,7 @@
         </is>
       </c>
       <c r="J3" s="79" t="n">
-        <v>0.167734845672019</v>
+        <v>0.1678566214990128</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -30963,7 +30963,7 @@
     </row>
     <row r="6">
       <c r="B6" s="2" t="n">
-        <v>0.58086156</v>
+        <v>0.58086225</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Automatic push - Update excel files
</commit_message>
<xml_diff>
--- a/Data/Historique d'achats.xlsx
+++ b/Data/Historique d'achats.xlsx
@@ -8197,7 +8197,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>2431.335117111788</v>
+        <v>2455.440521358299</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -8525,7 +8525,7 @@
     </row>
     <row r="12">
       <c r="B12" s="25" t="n">
-        <v>0.00709191</v>
+        <v>0.00710312</v>
       </c>
       <c r="C12" s="61" t="n">
         <v>0</v>
@@ -9349,7 +9349,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>1.395088987575467</v>
+        <v>1.396454906473141</v>
       </c>
     </row>
     <row r="4">
@@ -9451,7 +9451,7 @@
     </row>
     <row r="6">
       <c r="B6" s="81" t="n">
-        <v>0.5977881900000001</v>
+        <v>0.59803823</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -9732,7 +9732,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>9.503314883651584</v>
+        <v>9.602054282041697</v>
       </c>
     </row>
     <row r="4">
@@ -9827,7 +9827,7 @@
     </row>
     <row r="7">
       <c r="B7" s="81" t="n">
-        <v>0.02860224</v>
+        <v>0.02863838</v>
       </c>
       <c r="C7" s="61" t="n">
         <v>0</v>
@@ -9987,7 +9987,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>35.44784459991394</v>
+        <v>35.99589187856695</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -10106,7 +10106,7 @@
     </row>
     <row r="6">
       <c r="B6" s="25" t="n">
-        <v>0.01664801</v>
+        <v>0.01665289</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -10640,7 +10640,7 @@
         </is>
       </c>
       <c r="J3" s="82" t="n">
-        <v>0.003540437388861341</v>
+        <v>0.003570107878730294</v>
       </c>
     </row>
     <row r="4">
@@ -11007,7 +11007,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>307.7784804309184</v>
+        <v>320.295438372621</v>
       </c>
     </row>
     <row r="4">
@@ -11293,7 +11293,7 @@
     </row>
     <row r="10">
       <c r="B10" s="84" t="n">
-        <v>0.00264962</v>
+        <v>0.00265695</v>
       </c>
       <c r="C10" s="61" t="n">
         <v>0</v>
@@ -11602,7 +11602,7 @@
         </is>
       </c>
       <c r="J3" s="85" t="n">
-        <v>0.08001050228778817</v>
+        <v>0.08059867116433098</v>
       </c>
     </row>
     <row r="4">
@@ -11664,7 +11664,7 @@
     </row>
     <row r="6">
       <c r="B6" s="81" t="n">
-        <v>0.2888292</v>
+        <v>0.2890073</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -11838,7 +11838,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>6.936090082813577</v>
+        <v>7.054712854784725</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -11957,7 +11957,7 @@
     </row>
     <row r="6">
       <c r="B6" s="25" t="n">
-        <v>0.0783703</v>
+        <v>0.07846918999999999</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -12326,7 +12326,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>53.44442799810887</v>
+        <v>53.8587455733869</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -12431,7 +12431,7 @@
     </row>
     <row r="6">
       <c r="B6" s="25" t="n">
-        <v>0.00298707</v>
+        <v>0.00298793</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -12733,7 +12733,7 @@
         </is>
       </c>
       <c r="J3" s="79" t="n">
-        <v>0.1612753629890426</v>
+        <v>0.1633709195980486</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -13306,7 +13306,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>12.32566301716714</v>
+        <v>12.38411094106382</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -13422,7 +13422,7 @@
     </row>
     <row r="6">
       <c r="B6" s="2" t="n">
-        <v>0.00234442</v>
+        <v>0.00234548</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -13755,7 +13755,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>44225.23836018965</v>
+        <v>45367.77344325328</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -13846,7 +13846,7 @@
     </row>
     <row r="6">
       <c r="B6" s="25" t="n">
-        <v>0.00035475</v>
+        <v>0.00035483</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -15319,7 +15319,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>0.7105861771675925</v>
+        <v>0.7204578030538494</v>
       </c>
     </row>
     <row r="4">
@@ -15568,7 +15568,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>2.929678585441778</v>
+        <v>2.882716181745281</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -15684,7 +15684,7 @@
     </row>
     <row r="6">
       <c r="B6" s="2" t="n">
-        <v>0.01978558</v>
+        <v>0.01982078</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -15973,7 +15973,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>18.73806294101846</v>
+        <v>18.60439166681106</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -16089,7 +16089,7 @@
     </row>
     <row r="6">
       <c r="B6" s="2" t="n">
-        <v>0.00246001</v>
+        <v>0.00246186</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -16364,7 +16364,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>68.73090757338211</v>
+        <v>69.23306915665707</v>
       </c>
       <c r="N3" s="24" t="n"/>
       <c r="O3" s="59" t="n"/>
@@ -16458,7 +16458,7 @@
     </row>
     <row r="6">
       <c r="B6" s="2" t="n">
-        <v>0.00130824</v>
+        <v>0.00131054</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -16812,7 +16812,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>0.6608173586844314</v>
+        <v>0.6670329349310323</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -16886,7 +16886,7 @@
     </row>
     <row r="6">
       <c r="B6" s="84" t="n">
-        <v>0.0581337</v>
+        <v>0.05815786</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -17185,7 +17185,7 @@
         </is>
       </c>
       <c r="J3" s="67" t="n">
-        <v>0.0001083803173017418</v>
+        <v>0.000109284373783932</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -17604,7 +17604,7 @@
     </row>
     <row r="18">
       <c r="B18" s="81" t="n">
-        <v>4984.77854249</v>
+        <v>4987.94653639</v>
       </c>
       <c r="C18" s="61" t="n">
         <v>0</v>
@@ -18056,7 +18056,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>0.8320084746581266</v>
+        <v>0.8399181815720049</v>
       </c>
       <c r="N3" s="19" t="n"/>
       <c r="O3" s="59" t="n"/>
@@ -18155,7 +18155,7 @@
     </row>
     <row r="6">
       <c r="B6" s="20" t="n">
-        <v>0.32762569</v>
+        <v>0.32771566</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -18621,7 +18621,7 @@
         </is>
       </c>
       <c r="J3" s="79" t="n">
-        <v>0.02268818025768446</v>
+        <v>0.02267118039018598</v>
       </c>
     </row>
     <row r="4">
@@ -18688,7 +18688,7 @@
     </row>
     <row r="6">
       <c r="B6" s="81" t="n">
-        <v>0.06628315</v>
+        <v>0.06640105</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -18896,7 +18896,7 @@
         </is>
       </c>
       <c r="J3" s="79" t="n">
-        <v>1.18250092292378</v>
+        <v>1.204251221209786</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -19002,7 +19002,7 @@
     </row>
     <row r="6">
       <c r="B6" s="81" t="n">
-        <v>0.34820876</v>
+        <v>0.3483066</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -19404,7 +19404,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>2.883934190571152</v>
+        <v>2.993502154840577</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -19577,7 +19577,7 @@
     </row>
     <row r="7">
       <c r="B7" s="2" t="n">
-        <v>0.10241865</v>
+        <v>0.1024629</v>
       </c>
       <c r="C7" s="61" t="n">
         <v>0</v>
@@ -23580,7 +23580,7 @@
         </is>
       </c>
       <c r="J3" s="79" t="n">
-        <v>0.6274692954273903</v>
+        <v>0.6533231605370864</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -23686,7 +23686,7 @@
     </row>
     <row r="6">
       <c r="B6" s="81" t="n">
-        <v>0.07614136000000001</v>
+        <v>0.07616124000000001</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -23955,7 +23955,7 @@
         </is>
       </c>
       <c r="J3" s="88" t="n">
-        <v>9.065334467021332e-06</v>
+        <v>9.30433073930671e-06</v>
       </c>
     </row>
     <row r="4">
@@ -24020,7 +24020,7 @@
     </row>
     <row r="6">
       <c r="B6" s="23" t="n">
-        <v>270.44</v>
+        <v>270.93</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -24262,7 +24262,7 @@
         </is>
       </c>
       <c r="J3" s="82" t="n">
-        <v>0.003628865493773073</v>
+        <v>0.003706384594778053</v>
       </c>
     </row>
     <row r="4">
@@ -24486,7 +24486,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>100.5348418805912</v>
+        <v>104.4192268711736</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -25084,7 +25084,7 @@
     </row>
     <row r="17">
       <c r="B17" s="25" t="n">
-        <v>0.06440989</v>
+        <v>0.06443372999999999</v>
       </c>
       <c r="C17" s="61" t="n">
         <v>0</v>
@@ -25980,7 +25980,7 @@
         </is>
       </c>
       <c r="J3" s="79" t="n">
-        <v>0.124806874439672</v>
+        <v>0.1228859470999167</v>
       </c>
     </row>
     <row r="4">
@@ -26044,7 +26044,7 @@
     </row>
     <row r="6">
       <c r="B6" s="20" t="n">
-        <v>0.26185983</v>
+        <v>0.26219406</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -26270,7 +26270,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>6.44687536251554</v>
+        <v>6.388302508554606</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -26394,7 +26394,7 @@
     </row>
     <row r="6">
       <c r="B6" s="2" t="n">
-        <v>0.00271742</v>
+        <v>0.00271959</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -26694,7 +26694,7 @@
         </is>
       </c>
       <c r="J3" s="79" t="n">
-        <v>0.5129651902592521</v>
+        <v>0.5174253976447166</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -26800,7 +26800,7 @@
     </row>
     <row r="6">
       <c r="B6" s="20" t="n">
-        <v>0.85428951</v>
+        <v>0.85511783</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -27107,7 +27107,7 @@
         </is>
       </c>
       <c r="J3" s="79" t="n">
-        <v>18.68234781146852</v>
+        <v>20.34118714598716</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -27213,7 +27213,7 @@
     </row>
     <row r="6">
       <c r="B6" s="2" t="n">
-        <v>0.00314797</v>
+        <v>0.0032199</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -27459,7 +27459,7 @@
         </is>
       </c>
       <c r="J3" s="79" t="n">
-        <v>2.88121615495917</v>
+        <v>2.879080135798365</v>
       </c>
       <c r="N3" s="19" t="n"/>
       <c r="O3" s="86" t="n"/>
@@ -27551,7 +27551,7 @@
     </row>
     <row r="6">
       <c r="B6" s="2" t="n">
-        <v>0.0006475</v>
+        <v>0.0006594</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -27753,7 +27753,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>0.3374789294062976</v>
+        <v>0.34262934593142</v>
       </c>
     </row>
     <row r="4">
@@ -28193,7 +28193,7 @@
         </is>
       </c>
       <c r="J3" s="67" t="n">
-        <v>0.004137509500077404</v>
+        <v>0.004088022272973143</v>
       </c>
     </row>
     <row r="4">
@@ -30057,7 +30057,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>8.502654493311978</v>
+        <v>8.507751093431359</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -30170,7 +30170,7 @@
     </row>
     <row r="6">
       <c r="B6" s="2" t="n">
-        <v>2.263e-05</v>
+        <v>2.284e-05</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -30433,7 +30433,7 @@
         </is>
       </c>
       <c r="J3" s="58" t="n">
-        <v>0.4990858220731613</v>
+        <v>0.5329478767823665</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -30544,7 +30544,7 @@
     </row>
     <row r="6">
       <c r="B6" s="2" t="n">
-        <v>0.77146149</v>
+        <v>0.7722146</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>
@@ -30857,7 +30857,7 @@
         </is>
       </c>
       <c r="J3" s="79" t="n">
-        <v>0.1678566214990128</v>
+        <v>0.1695777351279782</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -30963,7 +30963,7 @@
     </row>
     <row r="6">
       <c r="B6" s="2" t="n">
-        <v>0.58086225</v>
+        <v>0.58111037</v>
       </c>
       <c r="C6" s="61" t="n">
         <v>0</v>

</xml_diff>